<commit_message>
210801 : added 임형준
</commit_message>
<xml_diff>
--- a/제출자 명단.xlsx
+++ b/제출자 명단.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleej\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://soongsilac-my.sharepoint.com/personal/aleejaehun_soongsil_ac_kr/Documents/jHoon_20201491/SPLUG/2021 SPLUG/준회원 대상 정회원 심사/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3440FF91-CD18-4E74-A5E6-E3E3B0017F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{3440FF91-CD18-4E74-A5E6-E3E3B0017F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCEB6B3C-C30A-4B57-AC7C-26744F8A928E}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{CEBE2EB6-E1A8-4B61-AAF0-1B3B5C57A9FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CEBE2EB6-E1A8-4B61-AAF0-1B3B5C57A9FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>컴퓨터학부</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,6 +157,22 @@
   </si>
   <si>
     <t>김황조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윈도우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴파일 불가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>makefile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conio.h ?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -190,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +216,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,20 +307,35 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,138 +652,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FA1DE7-392D-4B4B-93B2-D974C030462C}">
-  <dimension ref="B1:G23"/>
+  <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.625" customWidth="1"/>
     <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="D14" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="D16" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="D17" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="D20" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="2" t="s">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
+      <c r="D22" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>